<commit_message>
main file-call all the relevnt file
</commit_message>
<xml_diff>
--- a/FinelFiles/VQA_TestSet_Res.xlsx
+++ b/FinelFiles/VQA_TestSet_Res.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="293">
   <si>
     <t>Images</t>
   </si>
@@ -32,13 +32,16 @@
     <t>what show  cystic nature of giant occipital encephalocele with small amount of brain tissue?</t>
   </si>
   <si>
+    <t>ct</t>
+  </si>
+  <si>
+    <t>kjae-64-388-g001</t>
+  </si>
+  <si>
+    <t>what show a subarachnoid hematoma near l5?</t>
+  </si>
+  <si>
     <t>mri</t>
-  </si>
-  <si>
-    <t>kjae-64-388-g001</t>
-  </si>
-  <si>
-    <t>what show a subarachnoid hematoma near l5?</t>
   </si>
   <si>
     <t>AIAN-18-11-g002</t>
@@ -1277,26 +1280,26 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1304,32 +1307,32 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -1337,10 +1340,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -1348,43 +1351,43 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -1392,65 +1395,65 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -1458,32 +1461,32 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -1491,43 +1494,43 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
@@ -1535,21 +1538,21 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
         <v>5</v>
@@ -1557,43 +1560,43 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C29" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C30" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
         <v>5</v>
@@ -1601,10 +1604,10 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
@@ -1612,10 +1615,10 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
@@ -1623,10 +1626,10 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C35" t="s">
         <v>5</v>
@@ -1634,32 +1637,32 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C36" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C37" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
@@ -1667,10 +1670,10 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B39" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C39" t="s">
         <v>5</v>
@@ -1678,10 +1681,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C40" t="s">
         <v>5</v>
@@ -1689,10 +1692,10 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
@@ -1700,32 +1703,32 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C42" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B43" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C43" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B44" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C44" t="s">
         <v>5</v>
@@ -1733,43 +1736,43 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B45" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C45" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B46" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C46" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B47" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C47" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B48" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C48" t="s">
         <v>5</v>
@@ -1777,10 +1780,10 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C49" t="s">
         <v>5</v>
@@ -1788,21 +1791,21 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B50" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C50" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B51" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C51" t="s">
         <v>5</v>
@@ -1810,65 +1813,65 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B52" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C52" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B53" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C53" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B54" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C54" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B55" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C55" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B56" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C56" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B57" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C57" t="s">
         <v>5</v>
@@ -1876,10 +1879,10 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B58" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C58" t="s">
         <v>5</v>
@@ -1887,65 +1890,65 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B59" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C59" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B60" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C60" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B61" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C61" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B62" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C62" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B63" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C63" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B64" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C64" t="s">
         <v>5</v>
@@ -1953,43 +1956,43 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B65" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C65" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B66" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C66" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B67" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C67" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B68" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C68" t="s">
         <v>5</v>
@@ -1997,21 +2000,21 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B69" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C69" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B70" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C70" t="s">
         <v>5</v>
@@ -2019,10 +2022,10 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B71" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C71" t="s">
         <v>5</v>
@@ -2030,32 +2033,32 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B72" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C72" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B73" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C73" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B74" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C74" t="s">
         <v>5</v>
@@ -2063,32 +2066,32 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B75" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C75" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B76" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C76" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B77" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C77" t="s">
         <v>5</v>
@@ -2096,76 +2099,76 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B78" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C78" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B79" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C79" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B80" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C80" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B81" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C81" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B82" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C82" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B83" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C83" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B84" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C84" t="s">
         <v>5</v>
@@ -2173,76 +2176,76 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B85" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C85" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B86" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C86" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B87" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C87" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B88" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C88" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B89" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C89" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B90" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C90" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B91" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C91" t="s">
         <v>5</v>
@@ -2250,43 +2253,43 @@
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B92" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C92" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B93" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C93" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B94" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C94" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B95" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C95" t="s">
         <v>5</v>
@@ -2294,10 +2297,10 @@
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B96" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C96" t="s">
         <v>5</v>
@@ -2305,32 +2308,32 @@
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B97" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C97" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B98" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C98" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B99" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C99" t="s">
         <v>5</v>
@@ -2338,10 +2341,10 @@
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B100" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C100" t="s">
         <v>5</v>
@@ -2349,32 +2352,32 @@
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B101" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C101" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B102" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C102" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B103" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C103" t="s">
         <v>5</v>
@@ -2382,43 +2385,43 @@
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B104" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C104" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B105" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C105" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B106" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C106" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B107" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C107" t="s">
         <v>5</v>
@@ -2426,21 +2429,21 @@
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B108" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C108" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B109" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C109" t="s">
         <v>5</v>
@@ -2448,43 +2451,43 @@
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B110" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C110" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B111" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C111" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B112" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C112" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B113" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C113" t="s">
         <v>5</v>
@@ -2492,21 +2495,21 @@
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B114" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C114" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B115" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C115" t="s">
         <v>5</v>
@@ -2514,21 +2517,21 @@
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B116" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C116" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B117" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C117" t="s">
         <v>5</v>
@@ -2536,32 +2539,32 @@
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B118" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C118" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B119" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C119" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B120" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C120" t="s">
         <v>5</v>
@@ -2569,10 +2572,10 @@
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B121" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C121" t="s">
         <v>5</v>
@@ -2580,32 +2583,32 @@
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B122" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C122" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B123" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C123" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B124" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C124" t="s">
         <v>5</v>
@@ -2613,10 +2616,10 @@
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B125" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C125" t="s">
         <v>5</v>
@@ -2624,32 +2627,32 @@
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B126" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C126" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B127" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C127" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B128" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C128" t="s">
         <v>5</v>
@@ -2657,10 +2660,10 @@
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B129" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C129" t="s">
         <v>5</v>
@@ -2668,65 +2671,65 @@
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B130" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C130" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B131" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C131" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B132" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C132" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B133" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C133" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B134" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C134" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B135" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C135" t="s">
         <v>5</v>
@@ -2734,10 +2737,10 @@
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B136" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C136" t="s">
         <v>5</v>
@@ -2745,10 +2748,10 @@
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B137" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C137" t="s">
         <v>5</v>
@@ -2756,32 +2759,32 @@
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B138" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C138" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B139" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C139" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B140" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C140" t="s">
         <v>5</v>
@@ -2789,21 +2792,21 @@
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B141" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C141" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B142" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C142" t="s">
         <v>5</v>
@@ -2811,35 +2814,35 @@
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B143" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C143" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B144" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C144" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B145" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C145" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>